<commit_message>
Added files and changes required for deployment to heroku
</commit_message>
<xml_diff>
--- a/xlsx/loaddata.xlsx
+++ b/xlsx/loaddata.xlsx
@@ -3006,10 +3006,10 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="I27 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.14"/>
@@ -3086,10 +3086,10 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="I27 B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.41"/>
@@ -3284,10 +3284,10 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="1" sqref="I27 F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33.14"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="E3" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3360,7 +3360,7 @@
       </c>
       <c r="E4" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3379,7 +3379,7 @@
       </c>
       <c r="E5" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="E6" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="E7" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="E8" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3455,7 +3455,7 @@
       </c>
       <c r="E9" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3474,7 +3474,7 @@
       </c>
       <c r="E10" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="E11" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3531,7 +3531,7 @@
       </c>
       <c r="E13" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="E14" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="E15" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3588,7 +3588,7 @@
       </c>
       <c r="E16" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="E17" s="21" t="n">
         <f aca="false">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,10 +3638,10 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="1" sqref="I27 G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.14"/>
@@ -3909,10 +3909,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="I27 E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.14"/>
@@ -4016,10 +4016,10 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="I27 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.14"/>
@@ -4160,10 +4160,10 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="I27 E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.14"/>
@@ -4304,10 +4304,10 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="I27 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.85"/>
@@ -4383,10 +4383,10 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="I27 C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.85"/>
@@ -4462,10 +4462,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="I27 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
   </cols>
@@ -4522,10 +4522,10 @@
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>65</v>
@@ -4798,7 +4798,7 @@
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>65</v>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="H10" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>65</v>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>64</v>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>64</v>
@@ -4930,10 +4930,10 @@
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>64</v>
+        <v>3</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>65</v>
@@ -4963,10 +4963,10 @@
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>64</v>
+        <v>1</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>65</v>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>64</v>
@@ -5029,7 +5029,7 @@
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>64</v>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>64</v>
@@ -5128,10 +5128,10 @@
       </c>
       <c r="H19" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>64</v>
+        <v>3</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="J19" s="0" t="s">
         <v>65</v>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H20" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>64</v>
@@ -5194,7 +5194,7 @@
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>64</v>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="H22" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>64</v>
@@ -5260,7 +5260,7 @@
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" s="11" t="s">
         <v>64</v>
@@ -5293,7 +5293,7 @@
       </c>
       <c r="H24" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>64</v>
@@ -5326,10 +5326,10 @@
       </c>
       <c r="H25" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>64</v>
+        <v>2</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>65</v>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>64</v>
@@ -5392,10 +5392,10 @@
       </c>
       <c r="H27" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>64</v>
+        <v>4</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="J27" s="0" t="s">
         <v>65</v>
@@ -5425,7 +5425,7 @@
       </c>
       <c r="H28" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I28" s="11" t="s">
         <v>64</v>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="H32" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I32" s="11" t="s">
         <v>65</v>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="H33" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I33" s="11" t="s">
         <v>65</v>
@@ -5623,7 +5623,7 @@
       </c>
       <c r="H34" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I34" s="11" t="s">
         <v>65</v>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="H36" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>64</v>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="H37" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I37" s="11" t="s">
         <v>64</v>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="H38" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I38" s="11" t="s">
         <v>64</v>
@@ -5788,7 +5788,7 @@
       </c>
       <c r="H39" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I39" s="11" t="s">
         <v>64</v>
@@ -5821,7 +5821,7 @@
       </c>
       <c r="H40" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I40" s="11" t="s">
         <v>65</v>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="H41" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I41" s="11" t="s">
         <v>65</v>
@@ -5920,7 +5920,7 @@
       </c>
       <c r="H43" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I43" s="11" t="s">
         <v>65</v>
@@ -5953,7 +5953,7 @@
       </c>
       <c r="H44" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I44" s="11" t="s">
         <v>64</v>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="H45" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I45" s="11" t="s">
         <v>64</v>
@@ -6052,7 +6052,7 @@
       </c>
       <c r="H47" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47" s="11" t="s">
         <v>64</v>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="H48" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I48" s="11" t="s">
         <v>65</v>
@@ -6118,7 +6118,7 @@
       </c>
       <c r="H49" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I49" s="11" t="s">
         <v>65</v>
@@ -6151,7 +6151,7 @@
       </c>
       <c r="H50" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>65</v>
@@ -6184,7 +6184,7 @@
       </c>
       <c r="H51" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I51" s="11" t="s">
         <v>65</v>
@@ -6217,7 +6217,7 @@
       </c>
       <c r="H52" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>65</v>
@@ -6250,7 +6250,7 @@
       </c>
       <c r="H53" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>64</v>
@@ -6316,7 +6316,7 @@
       </c>
       <c r="H55" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I55" s="11" t="s">
         <v>64</v>
@@ -6349,7 +6349,7 @@
       </c>
       <c r="H56" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I56" s="11" t="s">
         <v>64</v>
@@ -6382,7 +6382,7 @@
       </c>
       <c r="H57" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>65</v>
@@ -6448,7 +6448,7 @@
       </c>
       <c r="H59" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I59" s="11" t="s">
         <v>65</v>
@@ -6514,7 +6514,7 @@
       </c>
       <c r="H61" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I61" s="11" t="s">
         <v>65</v>
@@ -6547,7 +6547,7 @@
       </c>
       <c r="H62" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I62" s="11" t="s">
         <v>65</v>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="H63" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I63" s="11" t="s">
         <v>65</v>
@@ -6613,7 +6613,7 @@
       </c>
       <c r="H64" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I64" s="11" t="s">
         <v>64</v>
@@ -6679,7 +6679,7 @@
       </c>
       <c r="H66" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I66" s="11" t="s">
         <v>64</v>
@@ -6712,7 +6712,7 @@
       </c>
       <c r="H67" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>64</v>
@@ -6745,7 +6745,7 @@
       </c>
       <c r="H68" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68" s="11" t="s">
         <v>65</v>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="H69" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I69" s="11" t="s">
         <v>65</v>
@@ -6844,7 +6844,7 @@
       </c>
       <c r="H71" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I71" s="11" t="s">
         <v>65</v>
@@ -6877,7 +6877,7 @@
       </c>
       <c r="H72" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I72" s="11" t="s">
         <v>64</v>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="H73" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I73" s="11" t="s">
         <v>64</v>
@@ -7009,7 +7009,7 @@
       </c>
       <c r="H76" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I76" s="11" t="s">
         <v>65</v>
@@ -7042,7 +7042,7 @@
       </c>
       <c r="H77" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I77" s="11" t="s">
         <v>65</v>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="H78" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I78" s="11" t="s">
         <v>65</v>
@@ -7108,7 +7108,7 @@
       </c>
       <c r="H79" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I79" s="11" t="s">
         <v>65</v>
@@ -7141,7 +7141,7 @@
       </c>
       <c r="H80" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>65</v>
@@ -7174,7 +7174,7 @@
       </c>
       <c r="H81" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I81" s="11" t="s">
         <v>65</v>
@@ -7207,7 +7207,7 @@
       </c>
       <c r="H82" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82" s="11" t="s">
         <v>65</v>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="H83" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I83" s="11" t="s">
         <v>65</v>
@@ -7273,7 +7273,7 @@
       </c>
       <c r="H84" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I84" s="11" t="s">
         <v>65</v>
@@ -7339,7 +7339,7 @@
       </c>
       <c r="H86" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I86" s="11" t="s">
         <v>65</v>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="H87" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I87" s="11" t="s">
         <v>65</v>
@@ -7405,7 +7405,7 @@
       </c>
       <c r="H88" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I88" s="11" t="s">
         <v>65</v>
@@ -7438,7 +7438,7 @@
       </c>
       <c r="H89" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I89" s="11" t="s">
         <v>65</v>
@@ -7504,7 +7504,7 @@
       </c>
       <c r="H91" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I91" s="11" t="s">
         <v>65</v>
@@ -7570,7 +7570,7 @@
       </c>
       <c r="H93" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I93" s="11" t="s">
         <v>65</v>
@@ -7603,7 +7603,7 @@
       </c>
       <c r="H94" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I94" s="11" t="s">
         <v>65</v>
@@ -7636,7 +7636,7 @@
       </c>
       <c r="H95" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I95" s="11" t="s">
         <v>65</v>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="H96" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>65</v>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="H98" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>65</v>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="H100" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I100" s="11" t="s">
         <v>65</v>
@@ -7834,7 +7834,7 @@
       </c>
       <c r="H101" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I101" s="11" t="s">
         <v>65</v>
@@ -7867,7 +7867,7 @@
       </c>
       <c r="H102" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I102" s="0" t="s">
         <v>64</v>
@@ -8003,10 +8003,10 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="I27 J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.28"/>
@@ -8075,15 +8075,15 @@
       </c>
       <c r="E3" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8109,11 +8109,11 @@
       </c>
       <c r="E4" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G4" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8143,23 +8143,23 @@
       </c>
       <c r="E5" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8177,19 +8177,19 @@
       </c>
       <c r="E6" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G6" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8211,11 +8211,11 @@
       </c>
       <c r="E7" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G7" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8223,7 +8223,7 @@
       </c>
       <c r="H7" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8245,23 +8245,23 @@
       </c>
       <c r="E8" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G8" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8273,7 +8273,7 @@
       </c>
       <c r="C9" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>1</v>
@@ -8284,7 +8284,7 @@
       </c>
       <c r="F9" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8296,7 +8296,7 @@
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8308,7 +8308,7 @@
       </c>
       <c r="C10" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>1</v>
@@ -8319,7 +8319,7 @@
       </c>
       <c r="F10" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G10" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8327,11 +8327,11 @@
       </c>
       <c r="H10" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8350,23 +8350,23 @@
       </c>
       <c r="E11" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G11" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8378,7 +8378,7 @@
       </c>
       <c r="C12" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>1</v>
@@ -8393,7 +8393,7 @@
       </c>
       <c r="G12" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8413,7 +8413,7 @@
       </c>
       <c r="C13" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>1</v>
@@ -8424,11 +8424,11 @@
       </c>
       <c r="F13" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G13" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8448,7 +8448,7 @@
       </c>
       <c r="C14" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>1</v>
@@ -8459,7 +8459,7 @@
       </c>
       <c r="F14" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8471,7 +8471,7 @@
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8483,18 +8483,18 @@
       </c>
       <c r="C15" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G15" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8502,7 +8502,7 @@
       </c>
       <c r="H15" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8518,14 +8518,14 @@
       </c>
       <c r="C16" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -8553,18 +8553,18 @@
       </c>
       <c r="C17" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G17" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8572,11 +8572,11 @@
       </c>
       <c r="H17" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8588,26 +8588,26 @@
       </c>
       <c r="C18" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G18" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8623,22 +8623,22 @@
       </c>
       <c r="C19" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G19" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8665,7 +8665,7 @@
       </c>
       <c r="E20" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F20" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -8673,15 +8673,15 @@
       </c>
       <c r="G20" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8693,22 +8693,22 @@
       </c>
       <c r="C21" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8728,18 +8728,18 @@
       </c>
       <c r="C22" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F22" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G22" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="I22" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8763,30 +8763,30 @@
       </c>
       <c r="C23" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G23" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8798,19 +8798,19 @@
       </c>
       <c r="C24" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>7</v>
+      </c>
+      <c r="E24" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
         <v>4</v>
       </c>
-      <c r="D24" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
-      </c>
       <c r="F24" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G24" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8818,7 +8818,7 @@
       </c>
       <c r="H24" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8834,19 +8834,19 @@
       </c>
       <c r="C25" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>6</v>
       </c>
-      <c r="D25" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
-      </c>
       <c r="E25" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F25" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G25" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8870,19 +8870,19 @@
       </c>
       <c r="C26" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G26" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8906,11 +8906,11 @@
       </c>
       <c r="C27" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D27" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E27" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -8922,7 +8922,7 @@
       </c>
       <c r="G27" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8930,7 +8930,7 @@
       </c>
       <c r="I27" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8942,11 +8942,11 @@
       </c>
       <c r="C28" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -8954,7 +8954,7 @@
       </c>
       <c r="F28" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G28" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -8962,11 +8962,11 @@
       </c>
       <c r="H28" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8978,23 +8978,23 @@
       </c>
       <c r="C29" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
+      <c r="D29" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>8</v>
+      </c>
+      <c r="E29" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>4</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>6</v>
       </c>
-      <c r="D29" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
-      </c>
-      <c r="E29" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
-      </c>
-      <c r="F29" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
-      </c>
       <c r="G29" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9002,7 +9002,7 @@
       </c>
       <c r="I29" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9014,11 +9014,11 @@
       </c>
       <c r="C30" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E30" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -9026,19 +9026,19 @@
       </c>
       <c r="F30" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G30" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9050,7 +9050,7 @@
       </c>
       <c r="C31" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D31" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -9058,23 +9058,23 @@
       </c>
       <c r="E31" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F31" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G31" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9086,31 +9086,31 @@
       </c>
       <c r="C32" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E32" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G32" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9122,11 +9122,11 @@
       </c>
       <c r="C33" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D33" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E33" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -9134,7 +9134,7 @@
       </c>
       <c r="F33" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G33" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9142,7 +9142,7 @@
       </c>
       <c r="H33" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9158,15 +9158,15 @@
       </c>
       <c r="C34" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E34" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -9174,15 +9174,15 @@
       </c>
       <c r="G34" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9194,31 +9194,31 @@
       </c>
       <c r="C35" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D35" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E35" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F35" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G35" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H35" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9230,7 +9230,7 @@
       </c>
       <c r="C36" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D36" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -9242,19 +9242,19 @@
       </c>
       <c r="F36" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G36" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9266,31 +9266,31 @@
       </c>
       <c r="C37" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E37" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F37" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G37" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I37" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9302,7 +9302,7 @@
       </c>
       <c r="C38" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D38" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -9310,11 +9310,11 @@
       </c>
       <c r="E38" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G38" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9322,7 +9322,7 @@
       </c>
       <c r="H38" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9342,27 +9342,27 @@
       </c>
       <c r="D39" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E39" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F39" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G39" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H39" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9374,23 +9374,23 @@
       </c>
       <c r="C40" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>7</v>
+      </c>
+      <c r="D40" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>3</v>
+      </c>
+      <c r="E40" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
         <v>4</v>
       </c>
-      <c r="D40" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
-      </c>
-      <c r="E40" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
-      </c>
       <c r="F40" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G40" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9398,7 +9398,7 @@
       </c>
       <c r="I40" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9410,7 +9410,7 @@
       </c>
       <c r="C41" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D41" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -9418,15 +9418,15 @@
       </c>
       <c r="E41" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F41" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G41" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H41" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9446,31 +9446,31 @@
       </c>
       <c r="C42" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
+      <c r="D42" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>10</v>
+      </c>
+      <c r="E42" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
         <v>3</v>
       </c>
-      <c r="D42" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
-      </c>
-      <c r="E42" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
-      </c>
       <c r="F42" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G42" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H42" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I42" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9486,15 +9486,15 @@
       </c>
       <c r="D43" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E43" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F43" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G43" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9502,7 +9502,7 @@
       </c>
       <c r="H43" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9518,20 +9518,20 @@
       </c>
       <c r="C44" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D44" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E44" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>3</v>
+      </c>
+      <c r="F44" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>4</v>
       </c>
-      <c r="F44" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
-      </c>
       <c r="G44" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
         <v>1</v>
@@ -9542,7 +9542,7 @@
       </c>
       <c r="I44" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9558,15 +9558,15 @@
       </c>
       <c r="D45" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E45" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G45" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9590,23 +9590,23 @@
       </c>
       <c r="C46" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D46" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E46" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G46" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H46" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9626,23 +9626,23 @@
       </c>
       <c r="C47" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D47" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>10</v>
+      </c>
+      <c r="E47" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>4</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>12</v>
       </c>
-      <c r="E47" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
-      </c>
-      <c r="F47" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
-      </c>
       <c r="G47" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9662,15 +9662,15 @@
       </c>
       <c r="C48" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D48" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E48" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F48" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -9678,11 +9678,11 @@
       </c>
       <c r="G48" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H48" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9698,31 +9698,31 @@
       </c>
       <c r="C49" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>2</v>
+      </c>
+      <c r="D49" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>7</v>
+      </c>
+      <c r="E49" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>1</v>
+      </c>
+      <c r="F49" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>5</v>
       </c>
-      <c r="D49" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
-      </c>
-      <c r="E49" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
-      </c>
-      <c r="F49" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
-      </c>
       <c r="G49" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
         <v>2</v>
       </c>
       <c r="H49" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9734,31 +9734,31 @@
       </c>
       <c r="C50" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
+      <c r="D50" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="F50" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>5</v>
       </c>
-      <c r="D50" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
-      </c>
-      <c r="E50" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
-      </c>
-      <c r="F50" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
-      </c>
       <c r="G50" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
         <v>2</v>
       </c>
       <c r="H50" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9770,11 +9770,11 @@
       </c>
       <c r="C51" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D51" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E51" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -9782,7 +9782,7 @@
       </c>
       <c r="F51" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G51" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9806,7 +9806,7 @@
       </c>
       <c r="C52" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D52" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -9814,15 +9814,15 @@
       </c>
       <c r="E52" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F52" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G52" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H52" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9830,7 +9830,7 @@
       </c>
       <c r="I52" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9842,23 +9842,23 @@
       </c>
       <c r="C53" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D53" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F53" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G53" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H53" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9866,7 +9866,7 @@
       </c>
       <c r="I53" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9878,11 +9878,11 @@
       </c>
       <c r="C54" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D54" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E54" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -9890,11 +9890,11 @@
       </c>
       <c r="F54" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G54" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H54" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9902,7 +9902,7 @@
       </c>
       <c r="I54" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9914,19 +9914,19 @@
       </c>
       <c r="C55" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D55" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E55" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F55" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9934,7 +9934,7 @@
       </c>
       <c r="H55" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9950,11 +9950,11 @@
       </c>
       <c r="C56" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E56" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -9962,7 +9962,7 @@
       </c>
       <c r="F56" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G56" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -9990,7 +9990,7 @@
       </c>
       <c r="D57" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E57" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -9998,19 +9998,19 @@
       </c>
       <c r="F57" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G57" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H57" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10022,11 +10022,11 @@
       </c>
       <c r="C58" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D58" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E58" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -10058,19 +10058,19 @@
       </c>
       <c r="C59" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D59" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E59" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F59" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G59" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10094,31 +10094,31 @@
       </c>
       <c r="C60" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="D60" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>7</v>
       </c>
-      <c r="D60" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
-      </c>
       <c r="E60" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F60" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G60" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10130,15 +10130,15 @@
       </c>
       <c r="C61" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E61" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F61" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -10146,11 +10146,11 @@
       </c>
       <c r="G61" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H61" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I61" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10170,15 +10170,15 @@
       </c>
       <c r="D62" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E62" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F62" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G62" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10186,11 +10186,11 @@
       </c>
       <c r="H62" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I62" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10202,19 +10202,19 @@
       </c>
       <c r="C63" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D63" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E63" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F63" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G63" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10226,7 +10226,7 @@
       </c>
       <c r="I63" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10238,23 +10238,23 @@
       </c>
       <c r="C64" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>2</v>
+      </c>
+      <c r="D64" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>6</v>
+      </c>
+      <c r="E64" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
         <v>4</v>
       </c>
-      <c r="D64" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
-      </c>
-      <c r="E64" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
-      </c>
       <c r="F64" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G64" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H64" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10274,19 +10274,19 @@
       </c>
       <c r="C65" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D65" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E65" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F65" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G65" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10310,23 +10310,23 @@
       </c>
       <c r="C66" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D66" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E66" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F66" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G66" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H66" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10346,31 +10346,31 @@
       </c>
       <c r="C67" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D67" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>10</v>
+      </c>
+      <c r="E67" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>4</v>
+      </c>
+      <c r="F67" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>11</v>
       </c>
-      <c r="E67" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
-      </c>
-      <c r="F67" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
-      </c>
       <c r="G67" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H67" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I67" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10382,23 +10382,23 @@
       </c>
       <c r="C68" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D68" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E68" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F68" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G68" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H68" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10406,7 +10406,7 @@
       </c>
       <c r="I68" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10418,11 +10418,11 @@
       </c>
       <c r="C69" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E69" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -10430,11 +10430,11 @@
       </c>
       <c r="F69" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G69" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H69" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10454,19 +10454,19 @@
       </c>
       <c r="C70" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D70" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E70" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F70" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G70" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10478,7 +10478,7 @@
       </c>
       <c r="I70" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10490,23 +10490,23 @@
       </c>
       <c r="C71" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D71" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E71" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F71" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G71" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H71" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10514,7 +10514,7 @@
       </c>
       <c r="I71" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10526,19 +10526,19 @@
       </c>
       <c r="C72" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D72" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E72" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F72" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G72" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10562,19 +10562,19 @@
       </c>
       <c r="C73" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E73" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F73" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G73" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10586,7 +10586,7 @@
       </c>
       <c r="I73" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10598,19 +10598,19 @@
       </c>
       <c r="C74" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D74" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E74" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F74" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G74" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10618,11 +10618,11 @@
       </c>
       <c r="H74" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I74" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10634,23 +10634,23 @@
       </c>
       <c r="C75" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="D75" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>5</v>
+      </c>
+      <c r="E75" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="F75" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>6</v>
       </c>
-      <c r="D75" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
-      </c>
-      <c r="E75" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
-      </c>
-      <c r="F75" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
-      </c>
       <c r="G75" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H75" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10658,7 +10658,7 @@
       </c>
       <c r="I75" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10670,27 +10670,27 @@
       </c>
       <c r="C76" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D76" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E76" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="F76" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>4</v>
       </c>
-      <c r="F76" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
-      </c>
       <c r="G76" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H76" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I76" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10710,15 +10710,15 @@
       </c>
       <c r="D77" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E77" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F77" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G77" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10726,7 +10726,7 @@
       </c>
       <c r="H77" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I77" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10742,19 +10742,19 @@
       </c>
       <c r="C78" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D78" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E78" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F78" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G78" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10762,7 +10762,7 @@
       </c>
       <c r="H78" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I78" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10778,31 +10778,31 @@
       </c>
       <c r="C79" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D79" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E79" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F79" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G79" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H79" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I79" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10814,11 +10814,11 @@
       </c>
       <c r="C80" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D80" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E80" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -10826,11 +10826,11 @@
       </c>
       <c r="F80" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G80" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H80" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10850,11 +10850,11 @@
       </c>
       <c r="C81" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D81" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E81" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -10862,11 +10862,11 @@
       </c>
       <c r="F81" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G81" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H81" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10874,7 +10874,7 @@
       </c>
       <c r="I81" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10890,15 +10890,15 @@
       </c>
       <c r="D82" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E82" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F82" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G82" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10926,15 +10926,15 @@
       </c>
       <c r="D83" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E83" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F83" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G83" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10958,19 +10958,19 @@
       </c>
       <c r="C84" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D84" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E84" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F84" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G84" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -10982,7 +10982,7 @@
       </c>
       <c r="I84" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10994,23 +10994,23 @@
       </c>
       <c r="C85" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
+      <c r="D85" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>12</v>
+      </c>
+      <c r="E85" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
         <v>3</v>
       </c>
-      <c r="D85" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
-      </c>
-      <c r="E85" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
-      </c>
       <c r="F85" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G85" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H85" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11030,11 +11030,11 @@
       </c>
       <c r="C86" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D86" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E86" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
@@ -11050,11 +11050,11 @@
       </c>
       <c r="H86" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I86" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11066,19 +11066,19 @@
       </c>
       <c r="C87" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D87" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E87" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G87" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11086,7 +11086,7 @@
       </c>
       <c r="H87" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I87" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11102,19 +11102,19 @@
       </c>
       <c r="C88" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D88" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E88" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G88" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11138,19 +11138,19 @@
       </c>
       <c r="C89" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F89" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G89" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11162,7 +11162,7 @@
       </c>
       <c r="I89" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11174,23 +11174,23 @@
       </c>
       <c r="C90" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="D90" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>4</v>
+      </c>
+      <c r="E90" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>1</v>
+      </c>
+      <c r="F90" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
         <v>6</v>
       </c>
-      <c r="D90" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
-      </c>
-      <c r="E90" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
-      </c>
-      <c r="F90" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
-      </c>
       <c r="G90" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H90" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11198,7 +11198,7 @@
       </c>
       <c r="I90" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11210,23 +11210,23 @@
       </c>
       <c r="C91" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="D91" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,12)</f>
+        <v>11</v>
+      </c>
+      <c r="E91" s="4" t="n">
+        <f aca="false">RANDBETWEEN(1,4)</f>
         <v>3</v>
       </c>
-      <c r="D91" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
-      </c>
-      <c r="E91" s="4" t="n">
-        <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
-      </c>
       <c r="F91" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G91" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H91" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11234,7 +11234,7 @@
       </c>
       <c r="I91" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11246,19 +11246,19 @@
       </c>
       <c r="C92" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D92" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E92" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G92" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11266,11 +11266,11 @@
       </c>
       <c r="H92" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I92" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11282,19 +11282,19 @@
       </c>
       <c r="C93" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D93" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E93" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F93" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G93" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11302,11 +11302,11 @@
       </c>
       <c r="H93" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I93" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11318,23 +11318,23 @@
       </c>
       <c r="C94" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D94" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E94" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F94" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G94" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H94" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11342,7 +11342,7 @@
       </c>
       <c r="I94" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11354,7 +11354,7 @@
       </c>
       <c r="C95" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D95" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -11362,11 +11362,11 @@
       </c>
       <c r="E95" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G95" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11374,11 +11374,11 @@
       </c>
       <c r="H95" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I95" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11394,11 +11394,11 @@
       </c>
       <c r="D96" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E96" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F96" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -11410,11 +11410,11 @@
       </c>
       <c r="H96" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I96" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11430,19 +11430,19 @@
       </c>
       <c r="D97" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E97" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F97" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G97" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H97" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11462,19 +11462,19 @@
       </c>
       <c r="C98" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D98" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E98" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F98" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G98" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11486,7 +11486,7 @@
       </c>
       <c r="I98" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11498,23 +11498,23 @@
       </c>
       <c r="C99" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D99" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E99" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F99" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G99" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H99" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11522,7 +11522,7 @@
       </c>
       <c r="I99" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11534,27 +11534,27 @@
       </c>
       <c r="C100" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D100" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E100" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F100" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G100" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H100" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11570,19 +11570,19 @@
       </c>
       <c r="C101" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D101" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E101" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F101" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G101" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
@@ -11594,7 +11594,7 @@
       </c>
       <c r="I101" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11610,19 +11610,19 @@
       </c>
       <c r="D102" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E102" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F102" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G102" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H102" s="4" t="n">
         <f aca="false">RANDBETWEEN(1,2)</f>

</xml_diff>